<commit_message>
Updating content to new structure
</commit_message>
<xml_diff>
--- a/identity-verification/module_1/media/IDVImageMapping.xlsx
+++ b/identity-verification/module_1/media/IDVImageMapping.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikames/Downloads/amazon-rekognition-code-samples-main-final/identity-verification/module_1/media/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buzecd/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7E57C1-A0B0-EC4D-A0CA-4534DA0930D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C14C0BB-AD3A-9B49-AE9F-3CE152A673C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{A3AFC66A-81CA-0841-B2AF-96395CB45576}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16140" xr2:uid="{A3AFC66A-81CA-0841-B2AF-96395CB45576}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="318">
   <si>
     <t>reference_name</t>
   </si>
@@ -969,6 +972,24 @@
   </si>
   <si>
     <t>Entity_X_Fish</t>
+  </si>
+  <si>
+    <t>Dani</t>
+  </si>
+  <si>
+    <t>dani.jpeg</t>
+  </si>
+  <si>
+    <t>dani_0.jpeg</t>
+  </si>
+  <si>
+    <t>dani_1.jpeg</t>
+  </si>
+  <si>
+    <t>dani_2.jpeg</t>
+  </si>
+  <si>
+    <t>dani_3.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1335,10 +1356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED0E4D9-E123-F543-B01A-2F132EE46ECF}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2388,7 +2409,32 @@
         <v>50</v>
       </c>
     </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" t="s">
+        <v>313</v>
+      </c>
+      <c r="C53" t="s">
+        <v>314</v>
+      </c>
+      <c r="D53" t="s">
+        <v>315</v>
+      </c>
+      <c r="E53" t="s">
+        <v>316</v>
+      </c>
+      <c r="F53" t="s">
+        <v>317</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{1ED0E4D9-E123-F543-B01A-2F132EE46ECF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F52">
+      <sortCondition ref="B1:B52"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F53">
     <sortCondition ref="B2:B53"/>
   </sortState>

</xml_diff>